<commit_message>
all instructions' control signal have done
</commit_message>
<xml_diff>
--- a/CPU24/单周期硬布线控制器表达式自动生成(2019-7-5) - 副本.xlsx
+++ b/CPU24/单周期硬布线控制器表达式自动生成(2019-7-5) - 副本.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -231,10 +231,10 @@
     <t>SLTU</t>
   </si>
   <si>
-    <t>J</t>
+    <t>X</t>
   </si>
   <si>
-    <t>X</t>
+    <t>J</t>
   </si>
   <si>
     <t>ADDI</t>
@@ -822,9 +822,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="49">
     <font>
@@ -985,7 +985,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1015,7 +1015,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1029,26 +1059,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1076,27 +1091,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1113,9 +1107,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1169,7 +1169,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1232,7 +1232,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1244,7 +1244,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1256,7 +1262,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1268,13 +1274,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1286,31 +1286,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1328,13 +1322,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1346,7 +1352,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1358,13 +1376,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,43 +1394,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1666,6 +1654,32 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1676,15 +1690,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1704,21 +1709,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1730,11 +1720,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1744,10 +1732,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="31" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="34" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1759,130 +1747,130 @@
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2416,7 +2404,7 @@
   <dimension ref="A1:AO61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2750,10 +2738,14 @@
       <c r="V3" s="27"/>
       <c r="W3" s="27"/>
       <c r="X3" s="27"/>
-      <c r="Y3" s="27"/>
+      <c r="Y3" s="27">
+        <v>1</v>
+      </c>
       <c r="Z3" s="27"/>
       <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
+      <c r="AB3" s="27">
+        <v>1</v>
+      </c>
       <c r="AC3" s="27"/>
       <c r="AD3" s="27"/>
       <c r="AE3" s="27"/>
@@ -2828,30 +2820,36 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="62" t="str">
+      <c r="Q4" s="61">
+        <v>2</v>
+      </c>
+      <c r="R4" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S4" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="S4" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T4" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="T4" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U4" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="U4" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V4" s="63"/>
       <c r="W4" s="63"/>
       <c r="X4" s="63"/>
-      <c r="Y4" s="63"/>
+      <c r="Y4" s="63">
+        <v>1</v>
+      </c>
       <c r="Z4" s="63"/>
       <c r="AA4" s="63"/>
-      <c r="AB4" s="63"/>
+      <c r="AB4" s="63">
+        <v>1</v>
+      </c>
       <c r="AC4" s="63"/>
       <c r="AD4" s="63"/>
       <c r="AE4" s="63"/>
@@ -2926,30 +2924,36 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="65" t="str">
+      <c r="Q5" s="64">
+        <v>5</v>
+      </c>
+      <c r="R5" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S5" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="S5" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T5" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="T5" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U5" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="U5" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V5" s="27"/>
       <c r="W5" s="27"/>
       <c r="X5" s="27"/>
-      <c r="Y5" s="27"/>
+      <c r="Y5" s="27">
+        <v>1</v>
+      </c>
       <c r="Z5" s="27"/>
       <c r="AA5" s="27"/>
-      <c r="AB5" s="27"/>
+      <c r="AB5" s="27">
+        <v>1</v>
+      </c>
       <c r="AC5" s="27"/>
       <c r="AD5" s="27"/>
       <c r="AE5" s="27"/>
@@ -3024,30 +3028,36 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="61"/>
-      <c r="R6" s="62" t="str">
+      <c r="Q6" s="61">
+        <v>5</v>
+      </c>
+      <c r="R6" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S6" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="S6" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T6" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="T6" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U6" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="U6" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V6" s="63"/>
       <c r="W6" s="63"/>
       <c r="X6" s="63"/>
-      <c r="Y6" s="63"/>
+      <c r="Y6" s="63">
+        <v>1</v>
+      </c>
       <c r="Z6" s="63"/>
       <c r="AA6" s="63"/>
-      <c r="AB6" s="63"/>
+      <c r="AB6" s="63">
+        <v>1</v>
+      </c>
       <c r="AC6" s="63"/>
       <c r="AD6" s="63"/>
       <c r="AE6" s="63"/>
@@ -3122,30 +3132,36 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="65" t="str">
+      <c r="Q7" s="64">
+        <v>6</v>
+      </c>
+      <c r="R7" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S7" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="S7" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T7" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="T7" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U7" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="U7" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V7" s="27"/>
       <c r="W7" s="27"/>
       <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
+      <c r="Y7" s="27">
+        <v>1</v>
+      </c>
       <c r="Z7" s="27"/>
       <c r="AA7" s="27"/>
-      <c r="AB7" s="27"/>
+      <c r="AB7" s="27">
+        <v>1</v>
+      </c>
       <c r="AC7" s="27"/>
       <c r="AD7" s="27"/>
       <c r="AE7" s="27"/>
@@ -3220,30 +3236,36 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="61"/>
-      <c r="R8" s="62" t="str">
+      <c r="Q8" s="61">
+        <v>7</v>
+      </c>
+      <c r="R8" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S8" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="S8" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T8" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="T8" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U8" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="U8" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V8" s="63"/>
       <c r="W8" s="63"/>
       <c r="X8" s="63"/>
-      <c r="Y8" s="63"/>
+      <c r="Y8" s="63">
+        <v>1</v>
+      </c>
       <c r="Z8" s="63"/>
       <c r="AA8" s="63"/>
-      <c r="AB8" s="63"/>
+      <c r="AB8" s="63">
+        <v>1</v>
+      </c>
       <c r="AC8" s="63"/>
       <c r="AD8" s="63"/>
       <c r="AE8" s="63"/>
@@ -3318,30 +3340,36 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="65" t="str">
+      <c r="Q9" s="64">
+        <v>8</v>
+      </c>
+      <c r="R9" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S9" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="S9" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T9" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="T9" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U9" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="U9" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V9" s="27"/>
       <c r="W9" s="27"/>
       <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
+      <c r="Y9" s="27">
+        <v>1</v>
+      </c>
       <c r="Z9" s="27"/>
       <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
+      <c r="AB9" s="27">
+        <v>1</v>
+      </c>
       <c r="AC9" s="27"/>
       <c r="AD9" s="27"/>
       <c r="AE9" s="27"/>
@@ -3416,30 +3444,36 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="62" t="str">
+      <c r="Q10" s="61">
+        <v>10</v>
+      </c>
+      <c r="R10" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S10" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="S10" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T10" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="T10" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U10" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="U10" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V10" s="63"/>
       <c r="W10" s="63"/>
       <c r="X10" s="63"/>
-      <c r="Y10" s="63"/>
+      <c r="Y10" s="63">
+        <v>1</v>
+      </c>
       <c r="Z10" s="63"/>
       <c r="AA10" s="63"/>
-      <c r="AB10" s="63"/>
+      <c r="AB10" s="63">
+        <v>1</v>
+      </c>
       <c r="AC10" s="63"/>
       <c r="AD10" s="63"/>
       <c r="AE10" s="63"/>
@@ -3514,30 +3548,36 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="64"/>
-      <c r="R11" s="65" t="str">
+      <c r="Q11" s="64">
+        <v>11</v>
+      </c>
+      <c r="R11" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S11" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="S11" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T11" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="T11" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U11" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="U11" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V11" s="27"/>
       <c r="W11" s="27"/>
       <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
+      <c r="Y11" s="27">
+        <v>1</v>
+      </c>
       <c r="Z11" s="27"/>
       <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
+      <c r="AB11" s="27">
+        <v>1</v>
+      </c>
       <c r="AC11" s="27"/>
       <c r="AD11" s="27"/>
       <c r="AE11" s="27"/>
@@ -3612,30 +3652,36 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="62" t="str">
+      <c r="Q12" s="61">
+        <v>12</v>
+      </c>
+      <c r="R12" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S12" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="S12" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T12" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="T12" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U12" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="U12" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V12" s="63"/>
       <c r="W12" s="63"/>
       <c r="X12" s="63"/>
-      <c r="Y12" s="63"/>
+      <c r="Y12" s="63">
+        <v>1</v>
+      </c>
       <c r="Z12" s="63"/>
       <c r="AA12" s="63"/>
-      <c r="AB12" s="63"/>
+      <c r="AB12" s="63">
+        <v>1</v>
+      </c>
       <c r="AC12" s="63"/>
       <c r="AD12" s="63"/>
       <c r="AE12" s="63"/>
@@ -3710,7 +3756,9 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="64"/>
+      <c r="Q13" s="64" t="s">
+        <v>46</v>
+      </c>
       <c r="R13" s="65" t="str">
         <f t="shared" si="12"/>
         <v>X</v>
@@ -3736,8 +3784,12 @@
       <c r="AB13" s="27"/>
       <c r="AC13" s="27"/>
       <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
+      <c r="AE13" s="27">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="27">
+        <v>1</v>
+      </c>
       <c r="AG13" s="27"/>
       <c r="AH13" s="28"/>
       <c r="AI13" s="28"/>
@@ -3829,7 +3881,9 @@
       <c r="W14" s="63"/>
       <c r="X14" s="63"/>
       <c r="Y14" s="63"/>
-      <c r="Z14" s="63"/>
+      <c r="Z14" s="63">
+        <v>1</v>
+      </c>
       <c r="AA14" s="63"/>
       <c r="AB14" s="63"/>
       <c r="AC14" s="63"/>
@@ -3850,13 +3904,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="28">
         <v>2</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="28">
         <f t="shared" si="0"/>
@@ -3906,7 +3960,9 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q15" s="64"/>
+      <c r="Q15" s="64" t="s">
+        <v>46</v>
+      </c>
       <c r="R15" s="65" t="str">
         <f t="shared" si="12"/>
         <v>X</v>
@@ -3933,7 +3989,9 @@
       <c r="AC15" s="27"/>
       <c r="AD15" s="27"/>
       <c r="AE15" s="27"/>
-      <c r="AF15" s="27"/>
+      <c r="AF15" s="27">
+        <v>1</v>
+      </c>
       <c r="AG15" s="27"/>
       <c r="AH15" s="28"/>
       <c r="AI15" s="28"/>
@@ -3954,7 +4012,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="0"/>
@@ -4004,7 +4062,9 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q16" s="61"/>
+      <c r="Q16" s="61" t="s">
+        <v>46</v>
+      </c>
       <c r="R16" s="62" t="str">
         <f t="shared" si="12"/>
         <v>X</v>
@@ -4031,8 +4091,12 @@
       <c r="AC16" s="63"/>
       <c r="AD16" s="63"/>
       <c r="AE16" s="63"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="23"/>
+      <c r="AF16" s="63">
+        <v>1</v>
+      </c>
+      <c r="AG16" s="23">
+        <v>1</v>
+      </c>
       <c r="AH16" s="24"/>
       <c r="AI16" s="24"/>
       <c r="AJ16" s="24"/>
@@ -4052,7 +4116,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" si="0"/>
@@ -4126,7 +4190,9 @@
       <c r="Z17" s="27"/>
       <c r="AA17" s="27"/>
       <c r="AB17" s="27"/>
-      <c r="AC17" s="27"/>
+      <c r="AC17" s="27">
+        <v>1</v>
+      </c>
       <c r="AD17" s="27"/>
       <c r="AE17" s="27"/>
       <c r="AF17" s="27"/>
@@ -4150,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="24">
         <f t="shared" si="0"/>
@@ -4225,7 +4291,9 @@
       <c r="AA18" s="63"/>
       <c r="AB18" s="63"/>
       <c r="AC18" s="63"/>
-      <c r="AD18" s="63"/>
+      <c r="AD18" s="63">
+        <v>1</v>
+      </c>
       <c r="AE18" s="63"/>
       <c r="AF18" s="63"/>
       <c r="AG18" s="23"/>
@@ -4248,7 +4316,7 @@
         <v>8</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="28">
         <f t="shared" si="0"/>
@@ -4298,29 +4366,37 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="65" t="str">
+      <c r="Q19" s="64">
+        <v>5</v>
+      </c>
+      <c r="R19" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S19" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="S19" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T19" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="T19" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U19" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="U19" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V19" s="27"/>
       <c r="W19" s="27"/>
-      <c r="X19" s="27"/>
-      <c r="Y19" s="27"/>
+      <c r="X19" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="27">
+        <v>1</v>
+      </c>
       <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
+      <c r="AA19" s="27">
+        <v>1</v>
+      </c>
       <c r="AB19" s="27"/>
       <c r="AC19" s="27"/>
       <c r="AD19" s="27"/>
@@ -4346,7 +4422,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="24">
         <f t="shared" si="0"/>
@@ -4396,27 +4472,33 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q20" s="61"/>
-      <c r="R20" s="62" t="str">
+      <c r="Q20" s="61">
+        <v>7</v>
+      </c>
+      <c r="R20" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S20" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="S20" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T20" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="T20" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U20" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="U20" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V20" s="63"/>
       <c r="W20" s="63"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="63"/>
+      <c r="X20" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="63">
+        <v>1</v>
+      </c>
       <c r="Z20" s="63"/>
       <c r="AA20" s="63"/>
       <c r="AB20" s="63"/>
@@ -4444,7 +4526,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="28">
         <f t="shared" si="0"/>
@@ -4494,29 +4576,37 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q21" s="64"/>
-      <c r="R21" s="65" t="str">
+      <c r="Q21" s="64">
+        <v>5</v>
+      </c>
+      <c r="R21" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S21" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="S21" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T21" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="T21" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U21" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="U21" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V21" s="27"/>
       <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
+      <c r="X21" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="27">
+        <v>1</v>
+      </c>
       <c r="Z21" s="27"/>
-      <c r="AA21" s="27"/>
+      <c r="AA21" s="27">
+        <v>1</v>
+      </c>
       <c r="AB21" s="27"/>
       <c r="AC21" s="27"/>
       <c r="AD21" s="27"/>
@@ -4542,7 +4632,7 @@
         <v>10</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="24">
         <f t="shared" si="0"/>
@@ -4592,29 +4682,37 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="62" t="str">
+      <c r="Q22" s="61">
+        <v>11</v>
+      </c>
+      <c r="R22" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S22" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="S22" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T22" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="T22" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U22" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="U22" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="V22" s="63"/>
       <c r="W22" s="63"/>
-      <c r="X22" s="63"/>
-      <c r="Y22" s="63"/>
+      <c r="X22" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="63">
+        <v>1</v>
+      </c>
       <c r="Z22" s="63"/>
-      <c r="AA22" s="63"/>
+      <c r="AA22" s="63">
+        <v>1</v>
+      </c>
       <c r="AB22" s="63"/>
       <c r="AC22" s="63"/>
       <c r="AD22" s="63"/>
@@ -4640,7 +4738,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" si="0"/>
@@ -4690,27 +4788,33 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="65" t="str">
+      <c r="Q23" s="64">
+        <v>8</v>
+      </c>
+      <c r="R23" s="65">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S23" s="65" t="str">
+        <v>1</v>
+      </c>
+      <c r="S23" s="65">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T23" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="T23" s="65">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U23" s="65" t="str">
+        <v>0</v>
+      </c>
+      <c r="U23" s="65">
         <f t="shared" si="15"/>
-        <v>X</v>
+        <v>0</v>
       </c>
       <c r="V23" s="27"/>
       <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="27"/>
+      <c r="X23" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="27">
+        <v>1</v>
+      </c>
       <c r="Z23" s="27"/>
       <c r="AA23" s="27"/>
       <c r="AB23" s="27"/>
@@ -4738,7 +4842,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="24">
         <f t="shared" si="0"/>
@@ -4788,29 +4892,39 @@
         <f t="shared" si="11"/>
         <v>X</v>
       </c>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="62" t="str">
+      <c r="Q24" s="61">
+        <v>5</v>
+      </c>
+      <c r="R24" s="62">
         <f t="shared" si="12"/>
-        <v>X</v>
-      </c>
-      <c r="S24" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="S24" s="62">
         <f t="shared" si="13"/>
-        <v>X</v>
-      </c>
-      <c r="T24" s="62" t="str">
+        <v>1</v>
+      </c>
+      <c r="T24" s="62">
         <f t="shared" si="14"/>
-        <v>X</v>
-      </c>
-      <c r="U24" s="62" t="str">
+        <v>0</v>
+      </c>
+      <c r="U24" s="62">
         <f t="shared" si="15"/>
-        <v>X</v>
-      </c>
-      <c r="V24" s="63"/>
+        <v>1</v>
+      </c>
+      <c r="V24" s="63">
+        <v>1</v>
+      </c>
       <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
+      <c r="X24" s="63">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="63">
+        <v>1</v>
+      </c>
       <c r="Z24" s="63"/>
-      <c r="AA24" s="63"/>
+      <c r="AA24" s="63">
+        <v>1</v>
+      </c>
       <c r="AB24" s="63"/>
       <c r="AC24" s="63"/>
       <c r="AD24" s="63"/>
@@ -4836,7 +4950,7 @@
         <v>43</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="28">
         <f t="shared" si="0"/>
@@ -4906,11 +5020,17 @@
         <v>1</v>
       </c>
       <c r="V25" s="27"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="27"/>
+      <c r="W25" s="27">
+        <v>1</v>
+      </c>
+      <c r="X25" s="27">
+        <v>1</v>
+      </c>
       <c r="Y25" s="27"/>
       <c r="Z25" s="27"/>
-      <c r="AA25" s="27"/>
+      <c r="AA25" s="27">
+        <v>1</v>
+      </c>
       <c r="AB25" s="27"/>
       <c r="AC25" s="27"/>
       <c r="AD25" s="27"/>
@@ -6984,7 +7104,7 @@
       </c>
       <c r="X3" s="37" t="str">
         <f>IF(真值表!Y3=1,$P3&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="Y3" s="37" t="str">
         <f>IF(真值表!Z3=1,$P3&amp;"+","")</f>
@@ -6996,7 +7116,7 @@
       </c>
       <c r="AA3" s="37" t="str">
         <f>IF(真值表!AB3=1,$P3&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AB3" s="37" t="str">
         <f>IF(真值表!AC3=1,$P3&amp;"+","")</f>
@@ -7122,7 +7242,7 @@
       </c>
       <c r="S4" s="37" t="str">
         <f>IF(真值表!T4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="T4" s="37" t="str">
         <f>IF(真值表!U4=1,$P4&amp;"+","")</f>
@@ -7142,7 +7262,7 @@
       </c>
       <c r="X4" s="37" t="str">
         <f>IF(真值表!Y4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="Y4" s="37" t="str">
         <f>IF(真值表!Z4=1,$P4&amp;"+","")</f>
@@ -7154,7 +7274,7 @@
       </c>
       <c r="AA4" s="37" t="str">
         <f>IF(真值表!AB4=1,$P4&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AB4" s="37" t="str">
         <f>IF(真值表!AC4=1,$P4&amp;"+","")</f>
@@ -7276,7 +7396,7 @@
       </c>
       <c r="R5" s="37" t="str">
         <f>IF(真值表!S5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="S5" s="37" t="str">
         <f>IF(真值表!T5=1,$P5&amp;"+","")</f>
@@ -7284,7 +7404,7 @@
       </c>
       <c r="T5" s="37" t="str">
         <f>IF(真值表!U5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="U5" s="37" t="str">
         <f>IF(真值表!V5=1,$P5&amp;"+","")</f>
@@ -7300,7 +7420,7 @@
       </c>
       <c r="X5" s="37" t="str">
         <f>IF(真值表!Y5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="Y5" s="37" t="str">
         <f>IF(真值表!Z5=1,$P5&amp;"+","")</f>
@@ -7312,7 +7432,7 @@
       </c>
       <c r="AA5" s="37" t="str">
         <f>IF(真值表!AB5=1,$P5&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AB5" s="37" t="str">
         <f>IF(真值表!AC5=1,$P5&amp;"+","")</f>
@@ -7434,7 +7554,7 @@
       </c>
       <c r="R6" s="37" t="str">
         <f>IF(真值表!S6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="S6" s="37" t="str">
         <f>IF(真值表!T6=1,$P6&amp;"+","")</f>
@@ -7442,7 +7562,7 @@
       </c>
       <c r="T6" s="37" t="str">
         <f>IF(真值表!U6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="U6" s="37" t="str">
         <f>IF(真值表!V6=1,$P6&amp;"+","")</f>
@@ -7458,7 +7578,7 @@
       </c>
       <c r="X6" s="37" t="str">
         <f>IF(真值表!Y6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="Y6" s="37" t="str">
         <f>IF(真值表!Z6=1,$P6&amp;"+","")</f>
@@ -7470,7 +7590,7 @@
       </c>
       <c r="AA6" s="37" t="str">
         <f>IF(真值表!AB6=1,$P6&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AB6" s="37" t="str">
         <f>IF(真值表!AC6=1,$P6&amp;"+","")</f>
@@ -7592,11 +7712,11 @@
       </c>
       <c r="R7" s="37" t="str">
         <f>IF(真值表!S7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="S7" s="37" t="str">
         <f>IF(真值表!T7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="T7" s="37" t="str">
         <f>IF(真值表!U7=1,$P7&amp;"+","")</f>
@@ -7616,7 +7736,7 @@
       </c>
       <c r="X7" s="37" t="str">
         <f>IF(真值表!Y7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="Y7" s="37" t="str">
         <f>IF(真值表!Z7=1,$P7&amp;"+","")</f>
@@ -7628,7 +7748,7 @@
       </c>
       <c r="AA7" s="37" t="str">
         <f>IF(真值表!AB7=1,$P7&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AB7" s="37" t="str">
         <f>IF(真值表!AC7=1,$P7&amp;"+","")</f>
@@ -7750,15 +7870,15 @@
       </c>
       <c r="R8" s="37" t="str">
         <f>IF(真值表!S8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="S8" s="37" t="str">
         <f>IF(真值表!T8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="T8" s="37" t="str">
         <f>IF(真值表!U8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="U8" s="37" t="str">
         <f>IF(真值表!V8=1,$P8&amp;"+","")</f>
@@ -7774,7 +7894,7 @@
       </c>
       <c r="X8" s="37" t="str">
         <f>IF(真值表!Y8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="Y8" s="37" t="str">
         <f>IF(真值表!Z8=1,$P8&amp;"+","")</f>
@@ -7786,7 +7906,7 @@
       </c>
       <c r="AA8" s="37" t="str">
         <f>IF(真值表!AB8=1,$P8&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AB8" s="37" t="str">
         <f>IF(真值表!AC8=1,$P8&amp;"+","")</f>
@@ -7904,7 +8024,7 @@
       </c>
       <c r="Q9" s="37" t="str">
         <f>IF(真值表!R9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="R9" s="37" t="str">
         <f>IF(真值表!S9=1,$P9&amp;"+","")</f>
@@ -7932,7 +8052,7 @@
       </c>
       <c r="X9" s="37" t="str">
         <f>IF(真值表!Y9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="Y9" s="37" t="str">
         <f>IF(真值表!Z9=1,$P9&amp;"+","")</f>
@@ -7944,7 +8064,7 @@
       </c>
       <c r="AA9" s="37" t="str">
         <f>IF(真值表!AB9=1,$P9&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+</v>
       </c>
       <c r="AB9" s="37" t="str">
         <f>IF(真值表!AC9=1,$P9&amp;"+","")</f>
@@ -8062,7 +8182,7 @@
       </c>
       <c r="Q10" s="37" t="str">
         <f>IF(真值表!R10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="R10" s="37" t="str">
         <f>IF(真值表!S10=1,$P10&amp;"+","")</f>
@@ -8070,7 +8190,7 @@
       </c>
       <c r="S10" s="37" t="str">
         <f>IF(真值表!T10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="T10" s="37" t="str">
         <f>IF(真值表!U10=1,$P10&amp;"+","")</f>
@@ -8090,7 +8210,7 @@
       </c>
       <c r="X10" s="37" t="str">
         <f>IF(真值表!Y10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="Y10" s="37" t="str">
         <f>IF(真值表!Z10=1,$P10&amp;"+","")</f>
@@ -8102,7 +8222,7 @@
       </c>
       <c r="AA10" s="37" t="str">
         <f>IF(真值表!AB10=1,$P10&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AB10" s="37" t="str">
         <f>IF(真值表!AC10=1,$P10&amp;"+","")</f>
@@ -8220,7 +8340,7 @@
       </c>
       <c r="Q11" s="37" t="str">
         <f>IF(真值表!R11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="R11" s="37" t="str">
         <f>IF(真值表!S11=1,$P11&amp;"+","")</f>
@@ -8228,11 +8348,11 @@
       </c>
       <c r="S11" s="37" t="str">
         <f>IF(真值表!T11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="T11" s="37" t="str">
         <f>IF(真值表!U11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="U11" s="37" t="str">
         <f>IF(真值表!V11=1,$P11&amp;"+","")</f>
@@ -8248,7 +8368,7 @@
       </c>
       <c r="X11" s="37" t="str">
         <f>IF(真值表!Y11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="Y11" s="37" t="str">
         <f>IF(真值表!Z11=1,$P11&amp;"+","")</f>
@@ -8260,7 +8380,7 @@
       </c>
       <c r="AA11" s="37" t="str">
         <f>IF(真值表!AB11=1,$P11&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+</v>
       </c>
       <c r="AB11" s="37" t="str">
         <f>IF(真值表!AC11=1,$P11&amp;"+","")</f>
@@ -8378,11 +8498,11 @@
       </c>
       <c r="Q12" s="37" t="str">
         <f>IF(真值表!R12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="R12" s="37" t="str">
         <f>IF(真值表!S12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="S12" s="37" t="str">
         <f>IF(真值表!T12=1,$P12&amp;"+","")</f>
@@ -8406,7 +8526,7 @@
       </c>
       <c r="X12" s="37" t="str">
         <f>IF(真值表!Y12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="Y12" s="37" t="str">
         <f>IF(真值表!Z12=1,$P12&amp;"+","")</f>
@@ -8418,7 +8538,7 @@
       </c>
       <c r="AA12" s="37" t="str">
         <f>IF(真值表!AB12=1,$P12&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AB12" s="37" t="str">
         <f>IF(真值表!AC12=1,$P12&amp;"+","")</f>
@@ -8588,11 +8708,11 @@
       </c>
       <c r="AD13" s="37" t="str">
         <f>IF(真值表!AE13=1,$P13&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AE13" s="37" t="str">
         <f>IF(真值表!AF13=1,$P13&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AF13" s="37" t="str">
         <f>IF(真值表!AG13=1,$P13&amp;"+","")</f>
@@ -8726,7 +8846,7 @@
       </c>
       <c r="Y14" s="37" t="str">
         <f>IF(真值表!Z14=1,$P14&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="Z14" s="37" t="str">
         <f>IF(真值表!AA14=1,$P14&amp;"+","")</f>
@@ -8908,7 +9028,7 @@
       </c>
       <c r="AE15" s="37" t="str">
         <f>IF(真值表!AF15=1,$P15&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="AF15" s="37" t="str">
         <f>IF(真值表!AG15=1,$P15&amp;"+","")</f>
@@ -9066,11 +9186,11 @@
       </c>
       <c r="AE16" s="37" t="str">
         <f>IF(真值表!AF16=1,$P16&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AF16" s="37" t="str">
         <f>IF(真值表!AG16=1,$P16&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AG16" s="37" t="str">
         <f>IF(真值表!AH16=1,$P16&amp;"+","")</f>
@@ -9212,7 +9332,7 @@
       </c>
       <c r="AB17" s="37" t="str">
         <f>IF(真值表!AC17=1,$P17&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AC17" s="37" t="str">
         <f>IF(真值表!AD17=1,$P17&amp;"+","")</f>
@@ -9374,7 +9494,7 @@
       </c>
       <c r="AC18" s="37" t="str">
         <f>IF(真值表!AD18=1,$P18&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AD18" s="37" t="str">
         <f>IF(真值表!AE18=1,$P18&amp;"+","")</f>
@@ -9488,7 +9608,7 @@
       </c>
       <c r="R19" s="37" t="str">
         <f>IF(真值表!S19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="S19" s="37" t="str">
         <f>IF(真值表!T19=1,$P19&amp;"+","")</f>
@@ -9496,7 +9616,7 @@
       </c>
       <c r="T19" s="37" t="str">
         <f>IF(真值表!U19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="U19" s="37" t="str">
         <f>IF(真值表!V19=1,$P19&amp;"+","")</f>
@@ -9508,11 +9628,11 @@
       </c>
       <c r="W19" s="37" t="str">
         <f>IF(真值表!X19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="X19" s="37" t="str">
         <f>IF(真值表!Y19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="Y19" s="37" t="str">
         <f>IF(真值表!Z19=1,$P19&amp;"+","")</f>
@@ -9520,7 +9640,7 @@
       </c>
       <c r="Z19" s="37" t="str">
         <f>IF(真值表!AA19=1,$P19&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AA19" s="37" t="str">
         <f>IF(真值表!AB19=1,$P19&amp;"+","")</f>
@@ -9646,15 +9766,15 @@
       </c>
       <c r="R20" s="37" t="str">
         <f>IF(真值表!S20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="S20" s="37" t="str">
         <f>IF(真值表!T20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="T20" s="37" t="str">
         <f>IF(真值表!U20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="U20" s="37" t="str">
         <f>IF(真值表!V20=1,$P20&amp;"+","")</f>
@@ -9666,11 +9786,11 @@
       </c>
       <c r="W20" s="37" t="str">
         <f>IF(真值表!X20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="X20" s="37" t="str">
         <f>IF(真值表!Y20=1,$P20&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="Y20" s="37" t="str">
         <f>IF(真值表!Z20=1,$P20&amp;"+","")</f>
@@ -9804,7 +9924,7 @@
       </c>
       <c r="R21" s="37" t="str">
         <f>IF(真值表!S21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="S21" s="37" t="str">
         <f>IF(真值表!T21=1,$P21&amp;"+","")</f>
@@ -9812,7 +9932,7 @@
       </c>
       <c r="T21" s="37" t="str">
         <f>IF(真值表!U21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="U21" s="37" t="str">
         <f>IF(真值表!V21=1,$P21&amp;"+","")</f>
@@ -9824,11 +9944,11 @@
       </c>
       <c r="W21" s="37" t="str">
         <f>IF(真值表!X21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="X21" s="37" t="str">
         <f>IF(真值表!Y21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="Y21" s="37" t="str">
         <f>IF(真值表!Z21=1,$P21&amp;"+","")</f>
@@ -9836,7 +9956,7 @@
       </c>
       <c r="Z21" s="37" t="str">
         <f>IF(真值表!AA21=1,$P21&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AA21" s="37" t="str">
         <f>IF(真值表!AB21=1,$P21&amp;"+","")</f>
@@ -9958,7 +10078,7 @@
       </c>
       <c r="Q22" s="37" t="str">
         <f>IF(真值表!R22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="R22" s="37" t="str">
         <f>IF(真值表!S22=1,$P22&amp;"+","")</f>
@@ -9966,11 +10086,11 @@
       </c>
       <c r="S22" s="37" t="str">
         <f>IF(真值表!T22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="T22" s="37" t="str">
         <f>IF(真值表!U22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="U22" s="37" t="str">
         <f>IF(真值表!V22=1,$P22&amp;"+","")</f>
@@ -9982,11 +10102,11 @@
       </c>
       <c r="W22" s="37" t="str">
         <f>IF(真值表!X22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="X22" s="37" t="str">
         <f>IF(真值表!Y22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="Y22" s="37" t="str">
         <f>IF(真值表!Z22=1,$P22&amp;"+","")</f>
@@ -9994,7 +10114,7 @@
       </c>
       <c r="Z22" s="37" t="str">
         <f>IF(真值表!AA22=1,$P22&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="AA22" s="37" t="str">
         <f>IF(真值表!AB22=1,$P22&amp;"+","")</f>
@@ -10116,7 +10236,7 @@
       </c>
       <c r="Q23" s="37" t="str">
         <f>IF(真值表!R23=1,$P23&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="R23" s="37" t="str">
         <f>IF(真值表!S23=1,$P23&amp;"+","")</f>
@@ -10140,11 +10260,11 @@
       </c>
       <c r="W23" s="37" t="str">
         <f>IF(真值表!X23=1,$P23&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="X23" s="37" t="str">
         <f>IF(真值表!Y23=1,$P23&amp;"+","")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="Y23" s="37" t="str">
         <f>IF(真值表!Z23=1,$P23&amp;"+","")</f>
@@ -10278,7 +10398,7 @@
       </c>
       <c r="R24" s="37" t="str">
         <f>IF(真值表!S24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="S24" s="37" t="str">
         <f>IF(真值表!T24=1,$P24&amp;"+","")</f>
@@ -10286,11 +10406,11 @@
       </c>
       <c r="T24" s="37" t="str">
         <f>IF(真值表!U24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="U24" s="37" t="str">
         <f>IF(真值表!V24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="V24" s="37" t="str">
         <f>IF(真值表!W24=1,$P24&amp;"+","")</f>
@@ -10298,11 +10418,11 @@
       </c>
       <c r="W24" s="37" t="str">
         <f>IF(真值表!X24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="X24" s="37" t="str">
         <f>IF(真值表!Y24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="Y24" s="37" t="str">
         <f>IF(真值表!Z24=1,$P24&amp;"+","")</f>
@@ -10310,7 +10430,7 @@
       </c>
       <c r="Z24" s="37" t="str">
         <f>IF(真值表!AA24=1,$P24&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AA24" s="37" t="str">
         <f>IF(真值表!AB24=1,$P24&amp;"+","")</f>
@@ -10452,11 +10572,11 @@
       </c>
       <c r="V25" s="37" t="str">
         <f>IF(真值表!W25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="W25" s="37" t="str">
         <f>IF(真值表!X25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="X25" s="37" t="str">
         <f>IF(真值表!Y25=1,$P25&amp;"+","")</f>
@@ -10468,7 +10588,7 @@
       </c>
       <c r="Z25" s="37" t="str">
         <f>IF(真值表!AA25=1,$P25&amp;"+","")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AA25" s="37" t="str">
         <f>IF(真值表!AB25=1,$P25&amp;"+","")</f>
@@ -18976,67 +19096,67 @@
       <c r="P82" s="39"/>
       <c r="Q82" s="40" t="str">
         <f t="shared" ref="Q82:T82" si="3">IF(LEN(Q83)&gt;1,LEFT(Q83,LEN(Q83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0</v>
       </c>
       <c r="R82" s="40" t="str">
         <f t="shared" si="3"/>
-        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="S82" s="40" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0</v>
       </c>
       <c r="T82" s="41" t="str">
         <f t="shared" si="3"/>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="U82" s="40" t="str">
         <f t="shared" ref="U82:X82" si="4">IF(LEN(U83)&gt;1,LEFT(U83,LEN(U83)-1),"")</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="V82" s="40" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="W82" s="41" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="X82" s="40" t="str">
         <f t="shared" si="4"/>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="Y82" s="40" t="str">
         <f t="shared" ref="Y82" si="5">IF(LEN(Y83)&gt;1,LEFT(Y83,LEN(Y83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0</v>
       </c>
       <c r="Z82" s="41" t="str">
         <f t="shared" ref="Z82" si="6">IF(LEN(Z83)&gt;1,LEFT(Z83,LEN(Z83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="AA82" s="40" t="str">
         <f t="shared" ref="AA82:AB82" si="7">IF(LEN(AA83)&gt;1,LEFT(AA83,LEN(AA83)-1),"")</f>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0</v>
       </c>
       <c r="AB82" s="40" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0</v>
       </c>
       <c r="AC82" s="40" t="str">
         <f t="shared" ref="AC82" si="8">IF(LEN(AC83)&gt;1,LEFT(AC83,LEN(AC83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0</v>
       </c>
       <c r="AD82" s="40" t="str">
         <f t="shared" ref="AD82" si="9">IF(LEN(AD83)&gt;1,LEFT(AD83,LEN(AD83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0</v>
       </c>
       <c r="AE82" s="41" t="str">
         <f t="shared" ref="AE82:AF82" si="10">IF(LEN(AE83)&gt;1,LEFT(AE83,LEN(AE83)-1),"")</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="AF82" s="42" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0</v>
       </c>
       <c r="AG82" s="40" t="str">
         <f t="shared" ref="AG82" si="11">IF(LEN(AG83)&gt;1,LEFT(AG83,LEN(AG83)-1),"")</f>
@@ -19070,67 +19190,67 @@
     <row r="83" hidden="1" spans="17:51">
       <c r="Q83" t="str">
         <f t="shared" ref="Q83:U83" si="17">CONCATENATE(Q2,Q3,Q4,Q5,Q6,Q7,Q8,Q9,Q10,Q11,Q12,Q13,Q14,Q15,Q16,Q17,Q18,Q19,Q20,Q21,Q22,Q23,Q24,Q25,Q26,Q27,Q28,Q29,Q30,Q31,Q32,Q33,Q34,Q35,Q36,Q37,Q38,Q39,Q40,Q41,Q42,Q43,Q44,Q45,Q46,Q47,Q48,Q49,Q50,Q51,Q52,Q53,Q54,Q55,Q56,Q57,)</f>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="R83" t="str">
         <f t="shared" si="17"/>
-        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="S83" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+</v>
       </c>
       <c r="T83" t="str">
         <f t="shared" si="17"/>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="U83" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v> OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="V83" t="str">
         <f t="shared" ref="V83:AY83" si="18">CONCATENATE(V2,V3,V4,V5,V6,V7,V8,V9,V10,V11,V12,V13,V14,V15,V16,V17,V18,V19,V20,V21,V22,V23,V24,V25,V26,V27,V28,V29,V30,V31,V32,V33,V34,V35,V36,V37,V38,V39,V40,V41,V42,V43,V44,V45,V46,V47,V48,V49,V50,V51,V52,V53,V54,V55,V56,V57,)</f>
-        <v/>
+        <v> OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="W83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="X83" t="str">
         <f t="shared" si="18"/>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp; OP2&amp;~OP1&amp; OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="Y83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp; F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="Z83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp;~OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp;~OP1&amp; OP0+~OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp;~OP0+ OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+ OP5&amp;~OP4&amp; OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AA83" t="str">
         <f t="shared" si="18"/>
-        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+</v>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp;~F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp;~F3&amp; F2&amp; F1&amp; F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp; F5&amp;~F4&amp; F3&amp;~F2&amp; F1&amp; F0+</v>
       </c>
       <c r="AB83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp;~OP0+</v>
       </c>
       <c r="AC83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp; OP2&amp;~OP1&amp; OP0+</v>
       </c>
       <c r="AD83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+</v>
       </c>
       <c r="AE83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp;~OP1&amp;~OP0&amp;~F5&amp;~F4&amp; F3&amp;~F2&amp;~F1&amp;~F0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp;~OP0+~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AF83" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>~OP5&amp;~OP4&amp;~OP3&amp;~OP2&amp; OP1&amp; OP0+</v>
       </c>
       <c r="AG83" t="str">
         <f t="shared" si="18"/>
@@ -19256,7 +19376,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="2"/>

</xml_diff>